<commit_message>
Changed recipes and consummption rate for reactor coolant and cores
</commit_message>
<xml_diff>
--- a/Info/recipes.xlsx
+++ b/Info/recipes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All_Programming_Projects\Satisfactory\Satisfactory_PostUpdate3\SF_Mod_RefinedPower\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE15D0-1C8D-4CCB-B269-70BF680D697C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EFDE87-625D-4ACC-8F96-327534DC5EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58500" yWindow="690" windowWidth="27120" windowHeight="14160" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Input</t>
   </si>
@@ -113,16 +113,13 @@
     <t>8000 (8m^3)</t>
   </si>
   <si>
-    <t>3000 (3m^3)</t>
-  </si>
-  <si>
     <t>1000 Cloudy Coolant</t>
   </si>
   <si>
-    <t>(change to 5000)</t>
-  </si>
-  <si>
     <t>1000 Water + 20 Coolant Powder</t>
+  </si>
+  <si>
+    <t>5000 (5m^3)</t>
   </si>
 </sst>
 </file>
@@ -612,7 +609,7 @@
   <dimension ref="B1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -809,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="16">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>12</v>
@@ -819,7 +816,7 @@
       </c>
       <c r="G12" s="20">
         <f>(60/D12)*F12</f>
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
@@ -832,13 +829,13 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="18">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>13</v>
@@ -848,7 +845,7 @@
       </c>
       <c r="G14" s="20">
         <f>(60/D14)*F14</f>
-        <v>2000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
@@ -861,7 +858,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>9</v>
@@ -883,17 +880,14 @@
         <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="D17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="J17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -901,7 +895,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -909,7 +903,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -917,7 +911,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -925,7 +919,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -933,7 +927,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -941,7 +935,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -949,7 +943,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -957,7 +951,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="C26" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed supplemental resource consumption and changed recipes to be more balanced
</commit_message>
<xml_diff>
--- a/Info/recipes.xlsx
+++ b/Info/recipes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All_Programming_Projects\Satisfactory\Satisfactory_PostUpdate3\SF_Mod_RefinedPower\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EFDE87-625D-4ACC-8F96-327534DC5EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F4AF28-450F-481C-BCC3-23E017FC272D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="28800" windowHeight="15460" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
+    <workbookView xWindow="5250" yWindow="3970" windowWidth="30140" windowHeight="11900" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Input</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Unfil Deuterium</t>
   </si>
   <si>
-    <t>Liquid Deuterium</t>
-  </si>
-  <si>
     <t>Adv Reactor Casing</t>
   </si>
   <si>
@@ -98,15 +95,9 @@
     <t>2 Limestone + 1 Coal + 2 Baux</t>
   </si>
   <si>
-    <t>4 Steel Beam + 4 Steel Pipe</t>
-  </si>
-  <si>
     <t>10000 Ref E65 + 10 Uranium</t>
   </si>
   <si>
-    <t>10000 Unfil Dueterium + 10000 water (10 packed water)</t>
-  </si>
-  <si>
     <t>1 Adv Reactor Casing + 2000 Liquid Deu</t>
   </si>
   <si>
@@ -120,6 +111,21 @@
   </si>
   <si>
     <t>5000 (5m^3)</t>
+  </si>
+  <si>
+    <t>10 Quartz Crystal + 1 Heavy Modular Frame</t>
+  </si>
+  <si>
+    <t>1000 Unfil Dueterium + 2000 water (2 packed water)</t>
+  </si>
+  <si>
+    <t>Liquid Deuterium + 2 empty canister</t>
+  </si>
+  <si>
+    <t>(enough output for 2 core production lines)</t>
+  </si>
+  <si>
+    <t>(enough output for 2 reactor coolant production lines)</t>
   </si>
 </sst>
 </file>
@@ -609,14 +615,17 @@
   <dimension ref="B1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="47.6328125" customWidth="1"/>
     <col min="3" max="3" width="26.90625" customWidth="1"/>
-    <col min="4" max="7" width="26.36328125" customWidth="1"/>
+    <col min="4" max="4" width="26.36328125" customWidth="1"/>
+    <col min="5" max="5" width="33.36328125" customWidth="1"/>
+    <col min="6" max="7" width="26.36328125" customWidth="1"/>
+    <col min="8" max="8" width="46.54296875" customWidth="1"/>
     <col min="9" max="9" width="26.6328125" customWidth="1"/>
     <col min="10" max="10" width="27.1796875" customWidth="1"/>
   </cols>
@@ -626,33 +635,33 @@
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="13">
         <v>3</v>
@@ -678,10 +687,10 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="13">
         <v>30</v>
@@ -707,23 +716,26 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="13">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F6" s="13">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="13">
         <f>(60/D6)*F6</f>
-        <v>10000</v>
+        <v>20000</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
@@ -736,23 +748,23 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="13">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="13">
         <v>1</v>
       </c>
       <c r="G8" s="13">
         <f>(60/D8)*F8</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
@@ -765,29 +777,29 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="13">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="F10" s="13">
         <v>1</v>
       </c>
       <c r="G10" s="13">
         <f>(60/D10)*F10</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I10">
         <v>375</v>
       </c>
       <c r="J10">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
@@ -800,23 +812,23 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16">
+        <v>3</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="D12" s="16">
-        <v>6</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="F12" s="20">
         <v>5</v>
       </c>
       <c r="G12" s="20">
         <f>(60/D12)*F12</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
@@ -829,23 +841,26 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D14" s="18">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="20">
         <v>1000</v>
       </c>
       <c r="G14" s="20">
         <f>(60/D14)*F14</f>
-        <v>2500</v>
+        <v>5000</v>
+      </c>
+      <c r="H14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
@@ -858,16 +873,16 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="18">
         <v>24</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F16" s="20">
         <v>1000</v>
@@ -877,10 +892,10 @@
         <v>2500</v>
       </c>
       <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
         <v>25</v>
-      </c>
-      <c r="J16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>